<commit_message>
passing iterations as a parameter
</commit_message>
<xml_diff>
--- a/analyze_application.xlsx
+++ b/analyze_application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo Poggiani\Documents\GitHub\WikiPageRank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B41C58-3E30-44F5-928C-57D59A7B4DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC17BE15-F45B-4300-87A9-B7A4EA3E43D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="792" windowWidth="17280" windowHeight="10044" xr2:uid="{048F8988-9BAE-4646-9C00-03FC07680F47}"/>
+    <workbookView minimized="1" xWindow="5496" yWindow="792" windowWidth="17280" windowHeight="10044" xr2:uid="{048F8988-9BAE-4646-9C00-03FC07680F47}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,33 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="27">
-  <si>
-    <t>Cache anche su ranks</t>
-  </si>
-  <si>
-    <t>Cache anche su contributions</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>Secondi</t>
-  </si>
-  <si>
-    <t>Cache su input</t>
-  </si>
-  <si>
-    <t>Cache anche su titles</t>
-  </si>
-  <si>
-    <t>Cache anche su ranks dentro for</t>
   </si>
   <si>
     <t>Con parallelize</t>
   </si>
   <si>
     <t>Senza parallelize</t>
-  </si>
-  <si>
-    <t>Senza cache</t>
   </si>
   <si>
     <t>1 iterazione</t>
@@ -115,6 +97,42 @@
   </si>
   <si>
     <t>Pr+A29:G39imi 5</t>
+  </si>
+  <si>
+    <t>Without cache</t>
+  </si>
+  <si>
+    <t>Cache only on the input</t>
+  </si>
+  <si>
+    <t>Cache also on titles</t>
+  </si>
+  <si>
+    <t>Cache also on ranks</t>
+  </si>
+  <si>
+    <t>Cache also on contributions</t>
+  </si>
+  <si>
+    <t>Cache inside for</t>
+  </si>
+  <si>
+    <t>1 iteration</t>
+  </si>
+  <si>
+    <t>2 iterations</t>
+  </si>
+  <si>
+    <t>5 iterations</t>
+  </si>
+  <si>
+    <t>10 iterations</t>
+  </si>
+  <si>
+    <t>20 iterations</t>
+  </si>
+  <si>
+    <t>100 iterations</t>
   </si>
 </sst>
 </file>
@@ -284,7 +302,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Cache</a:t>
+              <a:t>Analyzing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Cache (s)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -346,22 +372,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>Senza cache</c:v>
+                  <c:v>Without cache</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Cache su input</c:v>
+                  <c:v>Cache only on the input</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Cache anche su titles</c:v>
+                  <c:v>Cache also on titles</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Cache anche su ranks</c:v>
+                  <c:v>Cache also on ranks</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Cache anche su contributions</c:v>
+                  <c:v>Cache also on contributions</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Cache anche su ranks dentro for</c:v>
+                  <c:v>Cache inside for</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -612,11 +638,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tempo</a:t>
+              <a:t>Execution</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> di esecuzione</a:t>
+              <a:t> time (s)</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -759,22 +785,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1135,7 +1161,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Differenza di rank</a:t>
+              <a:t>Convergence of rankings</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1220,22 +1246,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1319,22 +1345,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1418,22 +1444,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1515,22 +1541,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1612,22 +1638,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1 iterazione</c:v>
+                  <c:v>1 iteration</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2 iterazioni</c:v>
+                  <c:v>2 iterations</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5 iterazioni</c:v>
+                  <c:v>5 iterations</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10 iterazioni</c:v>
+                  <c:v>10 iterations</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20 iterazioni</c:v>
+                  <c:v>20 iterations</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>100 iterazioni</c:v>
+                  <c:v>100 iterations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3595,14 +3621,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>179294</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>58271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1389529</xdr:colOff>
+      <xdr:colOff>1532963</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>112059</xdr:rowOff>
     </xdr:to>
@@ -3637,8 +3663,8 @@
       <xdr:rowOff>103093</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1891552</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>510988</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>89646</xdr:rowOff>
     </xdr:to>
@@ -3967,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31E5DA28-359C-40AF-8A84-3E6A0CD4C864}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3983,33 +4009,33 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C1" s="9"/>
     </row>
     <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -4034,10 +4060,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4050,27 +4076,27 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4096,7 +4122,7 @@
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4104,27 +4130,27 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B31">
         <v>1.8529668093948499E-3</v>
@@ -4150,27 +4176,27 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B33">
         <v>1.8259140482567899E-3</v>
@@ -4196,27 +4222,27 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B35">
         <v>1.7193307954166299E-3</v>
@@ -4242,27 +4268,27 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>1.69089068310794E-3</v>
@@ -4288,27 +4314,27 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>1.4661447603351099E-3</v>
@@ -4331,32 +4357,32 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F60" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -4385,27 +4411,27 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G63" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B64">
         <v>1.8529668093948399E-3</v>
@@ -4431,27 +4457,27 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B66">
         <v>1.8259140482567899E-3</v>
@@ -4477,27 +4503,27 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B68">
         <v>1.7193026240349401E-3</v>
@@ -4523,27 +4549,27 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G69" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B70">
         <v>1.6905845540935299E-3</v>
@@ -4569,27 +4595,27 @@
         <v>5</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G71" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B72">
         <v>1.4661447603351099E-3</v>

</xml_diff>